<commit_message>
reload bar chart data
</commit_message>
<xml_diff>
--- a/csv/data.xlsx
+++ b/csv/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DADABasefolder\dbproject\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{407A356D-7B54-4360-8D03-F43DA1E849FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A56474B-41DB-4AAE-A48C-15DCF62A8FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="5070" windowWidth="28800" windowHeight="15435" xr2:uid="{960C1731-0608-47ED-B164-B1125AB9A5EE}"/>
+    <workbookView xWindow="-28920" yWindow="8910" windowWidth="29040" windowHeight="15840" xr2:uid="{960C1731-0608-47ED-B164-B1125AB9A5EE}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -431,7 +431,7 @@
   <dimension ref="A1:BZ13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -680,232 +680,232 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D2">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E2">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="F2">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="G2">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="H2">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="I2">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="J2">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="K2">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="L2">
-        <v>18</v>
+        <v>95</v>
       </c>
       <c r="M2">
-        <v>20</v>
+        <v>98</v>
       </c>
       <c r="N2">
-        <v>21</v>
+        <v>109</v>
       </c>
       <c r="O2">
-        <v>23</v>
+        <v>113</v>
       </c>
       <c r="P2">
-        <v>26</v>
+        <v>123</v>
       </c>
       <c r="Q2">
-        <v>30</v>
+        <v>134</v>
       </c>
       <c r="R2">
-        <v>33</v>
+        <v>147</v>
       </c>
       <c r="S2">
-        <v>36</v>
+        <v>157</v>
       </c>
       <c r="T2">
-        <v>39</v>
+        <v>165</v>
       </c>
       <c r="U2">
-        <v>40</v>
+        <v>174</v>
       </c>
       <c r="V2">
-        <v>44</v>
+        <v>185</v>
       </c>
       <c r="W2">
-        <v>45</v>
+        <v>190</v>
       </c>
       <c r="X2">
-        <v>47</v>
+        <v>199</v>
       </c>
       <c r="Y2">
-        <v>50</v>
+        <v>207</v>
       </c>
       <c r="Z2">
-        <v>52</v>
+        <v>215</v>
       </c>
       <c r="AA2">
-        <v>52</v>
+        <v>220</v>
       </c>
       <c r="AB2">
-        <v>56</v>
+        <v>229</v>
       </c>
       <c r="AC2">
-        <v>57</v>
+        <v>237</v>
       </c>
       <c r="AD2">
-        <v>58</v>
+        <v>242</v>
       </c>
       <c r="AE2">
-        <v>58</v>
+        <v>248</v>
       </c>
       <c r="AF2">
-        <v>61</v>
+        <v>254</v>
       </c>
       <c r="AG2">
-        <v>65</v>
+        <v>260</v>
       </c>
       <c r="AH2">
-        <v>68</v>
+        <v>264</v>
       </c>
       <c r="AI2">
-        <v>69</v>
+        <v>274</v>
       </c>
       <c r="AJ2">
-        <v>70</v>
+        <v>281</v>
       </c>
       <c r="AK2">
-        <v>72</v>
+        <v>284</v>
       </c>
       <c r="AL2">
-        <v>74</v>
+        <v>294</v>
       </c>
       <c r="AM2">
-        <v>76</v>
+        <v>304</v>
       </c>
       <c r="AN2">
-        <v>77</v>
+        <v>312</v>
       </c>
       <c r="AO2">
-        <v>79</v>
+        <v>322</v>
       </c>
       <c r="AP2">
-        <v>80</v>
+        <v>327</v>
       </c>
       <c r="AQ2">
-        <v>82</v>
+        <v>333</v>
       </c>
       <c r="AR2">
-        <v>86</v>
+        <v>341</v>
       </c>
       <c r="AS2">
-        <v>91</v>
+        <v>354</v>
       </c>
       <c r="AT2">
-        <v>92</v>
+        <v>365</v>
       </c>
       <c r="AU2">
-        <v>92</v>
+        <v>372</v>
       </c>
       <c r="AV2">
-        <v>94</v>
+        <v>384</v>
       </c>
       <c r="AW2">
-        <v>98</v>
+        <v>400</v>
       </c>
       <c r="AX2">
-        <v>100</v>
+        <v>414</v>
       </c>
       <c r="AY2">
-        <v>104</v>
+        <v>434</v>
       </c>
       <c r="AZ2">
-        <v>108</v>
+        <v>445</v>
       </c>
       <c r="BA2">
-        <v>109</v>
+        <v>455</v>
       </c>
       <c r="BB2">
-        <v>112</v>
+        <v>462</v>
       </c>
       <c r="BC2">
-        <v>115</v>
+        <v>467</v>
       </c>
       <c r="BD2">
-        <v>118</v>
+        <v>477</v>
       </c>
       <c r="BE2">
-        <v>121</v>
+        <v>493</v>
       </c>
       <c r="BF2">
-        <v>122</v>
+        <v>505</v>
       </c>
       <c r="BG2">
-        <v>125</v>
+        <v>514</v>
       </c>
       <c r="BH2">
-        <v>129</v>
+        <v>524</v>
       </c>
       <c r="BI2">
-        <v>130</v>
+        <v>532</v>
       </c>
       <c r="BJ2">
-        <v>135</v>
+        <v>541</v>
       </c>
       <c r="BK2">
-        <v>135</v>
+        <v>545</v>
       </c>
       <c r="BL2">
-        <v>135</v>
+        <v>554</v>
       </c>
       <c r="BM2">
-        <v>137</v>
+        <v>565</v>
       </c>
       <c r="BN2">
-        <v>142</v>
+        <v>575</v>
       </c>
       <c r="BO2">
-        <v>144</v>
+        <v>588</v>
       </c>
       <c r="BP2">
-        <v>148</v>
+        <v>597</v>
       </c>
       <c r="BQ2">
-        <v>150</v>
+        <v>603</v>
       </c>
       <c r="BR2">
-        <v>154</v>
+        <v>616</v>
       </c>
       <c r="BS2">
-        <v>156</v>
+        <v>624</v>
       </c>
       <c r="BT2">
-        <v>157</v>
+        <v>627</v>
       </c>
       <c r="BU2">
-        <v>161</v>
+        <v>636</v>
       </c>
       <c r="BV2">
-        <v>161</v>
+        <v>638</v>
       </c>
       <c r="BW2">
-        <v>162</v>
+        <v>643</v>
       </c>
       <c r="BX2">
-        <v>165</v>
+        <v>648</v>
       </c>
       <c r="BY2">
-        <v>166</v>
+        <v>650</v>
       </c>
       <c r="BZ2">
-        <v>166</v>
+        <v>653</v>
       </c>
     </row>
     <row r="3" spans="1:78" x14ac:dyDescent="0.25">
@@ -916,232 +916,232 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D3">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="E3">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="F3">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="G3">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="H3">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="I3">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="J3">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="K3">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="L3">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="M3">
-        <v>16</v>
+        <v>85</v>
       </c>
       <c r="N3">
-        <v>17</v>
+        <v>93</v>
       </c>
       <c r="O3">
-        <v>19</v>
+        <v>102</v>
       </c>
       <c r="P3">
-        <v>20</v>
+        <v>108</v>
       </c>
       <c r="Q3">
-        <v>21</v>
+        <v>113</v>
       </c>
       <c r="R3">
-        <v>22</v>
+        <v>118</v>
       </c>
       <c r="S3">
-        <v>24</v>
+        <v>121</v>
       </c>
       <c r="T3">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="U3">
-        <v>33</v>
+        <v>136</v>
       </c>
       <c r="V3">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="W3">
-        <v>36</v>
+        <v>145</v>
       </c>
       <c r="X3">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="Y3">
-        <v>38</v>
+        <v>162</v>
       </c>
       <c r="Z3">
-        <v>45</v>
+        <v>171</v>
       </c>
       <c r="AA3">
-        <v>45</v>
+        <v>174</v>
       </c>
       <c r="AB3">
-        <v>46</v>
+        <v>177</v>
       </c>
       <c r="AC3">
-        <v>46</v>
+        <v>185</v>
       </c>
       <c r="AD3">
-        <v>47</v>
+        <v>188</v>
       </c>
       <c r="AE3">
-        <v>50</v>
+        <v>193</v>
       </c>
       <c r="AF3">
-        <v>51</v>
+        <v>196</v>
       </c>
       <c r="AG3">
-        <v>54</v>
+        <v>202</v>
       </c>
       <c r="AH3">
-        <v>56</v>
+        <v>208</v>
       </c>
       <c r="AI3">
-        <v>59</v>
+        <v>213</v>
       </c>
       <c r="AJ3">
-        <v>62</v>
+        <v>220</v>
       </c>
       <c r="AK3">
-        <v>63</v>
+        <v>226</v>
       </c>
       <c r="AL3">
-        <v>65</v>
+        <v>228</v>
       </c>
       <c r="AM3">
-        <v>66</v>
+        <v>230</v>
       </c>
       <c r="AN3">
-        <v>69</v>
+        <v>235</v>
       </c>
       <c r="AO3">
-        <v>71</v>
+        <v>239</v>
       </c>
       <c r="AP3">
-        <v>71</v>
+        <v>240</v>
       </c>
       <c r="AQ3">
-        <v>72</v>
+        <v>247</v>
       </c>
       <c r="AR3">
-        <v>74</v>
+        <v>257</v>
       </c>
       <c r="AS3">
-        <v>74</v>
+        <v>259</v>
       </c>
       <c r="AT3">
-        <v>75</v>
+        <v>266</v>
       </c>
       <c r="AU3">
-        <v>77</v>
+        <v>273</v>
       </c>
       <c r="AV3">
-        <v>77</v>
+        <v>278</v>
       </c>
       <c r="AW3">
-        <v>77</v>
+        <v>280</v>
       </c>
       <c r="AX3">
-        <v>78</v>
+        <v>287</v>
       </c>
       <c r="AY3">
-        <v>78</v>
+        <v>291</v>
       </c>
       <c r="AZ3">
-        <v>79</v>
+        <v>293</v>
       </c>
       <c r="BA3">
-        <v>81</v>
+        <v>295</v>
       </c>
       <c r="BB3">
-        <v>84</v>
+        <v>302</v>
       </c>
       <c r="BC3">
-        <v>86</v>
+        <v>305</v>
       </c>
       <c r="BD3">
-        <v>87</v>
+        <v>307</v>
       </c>
       <c r="BE3">
-        <v>88</v>
+        <v>311</v>
       </c>
       <c r="BF3">
-        <v>91</v>
+        <v>317</v>
       </c>
       <c r="BG3">
-        <v>92</v>
+        <v>319</v>
       </c>
       <c r="BH3">
-        <v>93</v>
+        <v>320</v>
       </c>
       <c r="BI3">
-        <v>96</v>
+        <v>324</v>
       </c>
       <c r="BJ3">
-        <v>99</v>
+        <v>327</v>
       </c>
       <c r="BK3">
-        <v>100</v>
+        <v>332</v>
       </c>
       <c r="BL3">
-        <v>103</v>
+        <v>336</v>
       </c>
       <c r="BM3">
-        <v>103</v>
+        <v>342</v>
       </c>
       <c r="BN3">
-        <v>103</v>
+        <v>345</v>
       </c>
       <c r="BO3">
-        <v>103</v>
+        <v>348</v>
       </c>
       <c r="BP3">
-        <v>105</v>
+        <v>350</v>
       </c>
       <c r="BQ3">
-        <v>107</v>
+        <v>353</v>
       </c>
       <c r="BR3">
-        <v>112</v>
+        <v>361</v>
       </c>
       <c r="BS3">
-        <v>112</v>
+        <v>361</v>
       </c>
       <c r="BT3">
-        <v>112</v>
+        <v>362</v>
       </c>
       <c r="BU3">
-        <v>116</v>
+        <v>368</v>
       </c>
       <c r="BV3">
-        <v>121</v>
+        <v>376</v>
       </c>
       <c r="BW3">
-        <v>124</v>
+        <v>379</v>
       </c>
       <c r="BX3">
-        <v>125</v>
+        <v>381</v>
       </c>
       <c r="BY3">
-        <v>125</v>
+        <v>381</v>
       </c>
       <c r="BZ3">
-        <v>125</v>
+        <v>381</v>
       </c>
     </row>
     <row r="4" spans="1:78" x14ac:dyDescent="0.25">
@@ -1152,232 +1152,232 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="E4">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="F4">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="G4">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="H4">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="I4">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="J4">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="K4">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="L4">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="M4">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="N4">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="O4">
-        <v>29</v>
+        <v>95</v>
       </c>
       <c r="P4">
-        <v>31</v>
+        <v>99</v>
       </c>
       <c r="Q4">
-        <v>33</v>
+        <v>103</v>
       </c>
       <c r="R4">
-        <v>34</v>
+        <v>108</v>
       </c>
       <c r="S4">
-        <v>35</v>
+        <v>112</v>
       </c>
       <c r="T4">
-        <v>37</v>
+        <v>120</v>
       </c>
       <c r="U4">
-        <v>41</v>
+        <v>127</v>
       </c>
       <c r="V4">
-        <v>47</v>
+        <v>137</v>
       </c>
       <c r="W4">
-        <v>49</v>
+        <v>143</v>
       </c>
       <c r="X4">
-        <v>56</v>
+        <v>155</v>
       </c>
       <c r="Y4">
-        <v>65</v>
+        <v>171</v>
       </c>
       <c r="Z4">
-        <v>69</v>
+        <v>179</v>
       </c>
       <c r="AA4">
-        <v>73</v>
+        <v>188</v>
       </c>
       <c r="AB4">
-        <v>80</v>
+        <v>200</v>
       </c>
       <c r="AC4">
-        <v>82</v>
+        <v>203</v>
       </c>
       <c r="AD4">
-        <v>82</v>
+        <v>209</v>
       </c>
       <c r="AE4">
-        <v>84</v>
+        <v>214</v>
       </c>
       <c r="AF4">
-        <v>87</v>
+        <v>219</v>
       </c>
       <c r="AG4">
-        <v>92</v>
+        <v>225</v>
       </c>
       <c r="AH4">
-        <v>96</v>
+        <v>233</v>
       </c>
       <c r="AI4">
-        <v>101</v>
+        <v>239</v>
       </c>
       <c r="AJ4">
-        <v>103</v>
+        <v>242</v>
       </c>
       <c r="AK4">
-        <v>104</v>
+        <v>248</v>
       </c>
       <c r="AL4">
-        <v>108</v>
+        <v>255</v>
       </c>
       <c r="AM4">
-        <v>110</v>
+        <v>261</v>
       </c>
       <c r="AN4">
-        <v>111</v>
+        <v>265</v>
       </c>
       <c r="AO4">
-        <v>112</v>
+        <v>272</v>
       </c>
       <c r="AP4">
-        <v>112</v>
+        <v>276</v>
       </c>
       <c r="AQ4">
-        <v>112</v>
+        <v>283</v>
       </c>
       <c r="AR4">
-        <v>112</v>
+        <v>285</v>
       </c>
       <c r="AS4">
-        <v>112</v>
+        <v>290</v>
       </c>
       <c r="AT4">
-        <v>114</v>
+        <v>296</v>
       </c>
       <c r="AU4">
-        <v>116</v>
+        <v>300</v>
       </c>
       <c r="AV4">
-        <v>117</v>
+        <v>308</v>
       </c>
       <c r="AW4">
-        <v>117</v>
+        <v>310</v>
       </c>
       <c r="AX4">
-        <v>119</v>
+        <v>314</v>
       </c>
       <c r="AY4">
-        <v>120</v>
+        <v>316</v>
       </c>
       <c r="AZ4">
-        <v>121</v>
+        <v>320</v>
       </c>
       <c r="BA4">
-        <v>124</v>
+        <v>324</v>
       </c>
       <c r="BB4">
-        <v>124</v>
+        <v>326</v>
       </c>
       <c r="BC4">
-        <v>126</v>
+        <v>330</v>
       </c>
       <c r="BD4">
-        <v>131</v>
+        <v>338</v>
       </c>
       <c r="BE4">
-        <v>134</v>
+        <v>346</v>
       </c>
       <c r="BF4">
-        <v>135</v>
+        <v>351</v>
       </c>
       <c r="BG4">
-        <v>138</v>
+        <v>361</v>
       </c>
       <c r="BH4">
-        <v>143</v>
+        <v>373</v>
       </c>
       <c r="BI4">
-        <v>144</v>
+        <v>378</v>
       </c>
       <c r="BJ4">
-        <v>145</v>
+        <v>380</v>
       </c>
       <c r="BK4">
-        <v>146</v>
+        <v>386</v>
       </c>
       <c r="BL4">
-        <v>147</v>
+        <v>390</v>
       </c>
       <c r="BM4">
-        <v>147</v>
+        <v>392</v>
       </c>
       <c r="BN4">
-        <v>150</v>
+        <v>396</v>
       </c>
       <c r="BO4">
-        <v>155</v>
+        <v>403</v>
       </c>
       <c r="BP4">
-        <v>157</v>
+        <v>407</v>
       </c>
       <c r="BQ4">
-        <v>158</v>
+        <v>410</v>
       </c>
       <c r="BR4">
-        <v>160</v>
+        <v>413</v>
       </c>
       <c r="BS4">
-        <v>160</v>
+        <v>414</v>
       </c>
       <c r="BT4">
-        <v>160</v>
+        <v>414</v>
       </c>
       <c r="BU4">
-        <v>162</v>
+        <v>416</v>
       </c>
       <c r="BV4">
-        <v>162</v>
+        <v>416</v>
       </c>
       <c r="BW4">
-        <v>164</v>
+        <v>419</v>
       </c>
       <c r="BX4">
-        <v>165</v>
+        <v>423</v>
       </c>
       <c r="BY4">
-        <v>167</v>
+        <v>425</v>
       </c>
       <c r="BZ4">
-        <v>168</v>
+        <v>428</v>
       </c>
     </row>
     <row r="5" spans="1:78" x14ac:dyDescent="0.25">
@@ -1388,232 +1388,232 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D5">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E5">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="F5">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="G5">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="H5">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="I5">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="J5">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="K5">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="L5">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="M5">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="N5">
-        <v>60</v>
+        <v>104</v>
       </c>
       <c r="O5">
-        <v>63</v>
+        <v>114</v>
       </c>
       <c r="P5">
-        <v>66</v>
+        <v>122</v>
       </c>
       <c r="Q5">
-        <v>70</v>
+        <v>131</v>
       </c>
       <c r="R5">
-        <v>75</v>
+        <v>141</v>
       </c>
       <c r="S5">
-        <v>81</v>
+        <v>155</v>
       </c>
       <c r="T5">
-        <v>93</v>
+        <v>174</v>
       </c>
       <c r="U5">
-        <v>97</v>
+        <v>180</v>
       </c>
       <c r="V5">
-        <v>106</v>
+        <v>194</v>
       </c>
       <c r="W5">
-        <v>112</v>
+        <v>207</v>
       </c>
       <c r="X5">
-        <v>119</v>
+        <v>221</v>
       </c>
       <c r="Y5">
-        <v>129</v>
+        <v>235</v>
       </c>
       <c r="Z5">
-        <v>133</v>
+        <v>248</v>
       </c>
       <c r="AA5">
-        <v>141</v>
+        <v>259</v>
       </c>
       <c r="AB5">
-        <v>148</v>
+        <v>270</v>
       </c>
       <c r="AC5">
-        <v>152</v>
+        <v>280</v>
       </c>
       <c r="AD5">
-        <v>160</v>
+        <v>293</v>
       </c>
       <c r="AE5">
-        <v>162</v>
+        <v>299</v>
       </c>
       <c r="AF5">
-        <v>169</v>
+        <v>311</v>
       </c>
       <c r="AG5">
-        <v>176</v>
+        <v>322</v>
       </c>
       <c r="AH5">
-        <v>185</v>
+        <v>339</v>
       </c>
       <c r="AI5">
-        <v>191</v>
+        <v>350</v>
       </c>
       <c r="AJ5">
-        <v>196</v>
+        <v>359</v>
       </c>
       <c r="AK5">
-        <v>200</v>
+        <v>369</v>
       </c>
       <c r="AL5">
-        <v>209</v>
+        <v>381</v>
       </c>
       <c r="AM5">
-        <v>210</v>
+        <v>384</v>
       </c>
       <c r="AN5">
-        <v>213</v>
+        <v>392</v>
       </c>
       <c r="AO5">
-        <v>215</v>
+        <v>405</v>
       </c>
       <c r="AP5">
-        <v>219</v>
+        <v>415</v>
       </c>
       <c r="AQ5">
-        <v>229</v>
+        <v>429</v>
       </c>
       <c r="AR5">
-        <v>232</v>
+        <v>440</v>
       </c>
       <c r="AS5">
-        <v>235</v>
+        <v>455</v>
       </c>
       <c r="AT5">
-        <v>242</v>
+        <v>479</v>
       </c>
       <c r="AU5">
-        <v>250</v>
+        <v>493</v>
       </c>
       <c r="AV5">
-        <v>255</v>
+        <v>503</v>
       </c>
       <c r="AW5">
-        <v>264</v>
+        <v>520</v>
       </c>
       <c r="AX5">
-        <v>268</v>
+        <v>533</v>
       </c>
       <c r="AY5">
-        <v>271</v>
+        <v>542</v>
       </c>
       <c r="AZ5">
-        <v>275</v>
+        <v>549</v>
       </c>
       <c r="BA5">
-        <v>281</v>
+        <v>559</v>
       </c>
       <c r="BB5">
-        <v>289</v>
+        <v>573</v>
       </c>
       <c r="BC5">
-        <v>296</v>
+        <v>584</v>
       </c>
       <c r="BD5">
-        <v>302</v>
+        <v>593</v>
       </c>
       <c r="BE5">
-        <v>309</v>
+        <v>609</v>
       </c>
       <c r="BF5">
-        <v>314</v>
+        <v>619</v>
       </c>
       <c r="BG5">
-        <v>319</v>
+        <v>629</v>
       </c>
       <c r="BH5">
-        <v>326</v>
+        <v>644</v>
       </c>
       <c r="BI5">
-        <v>331</v>
+        <v>654</v>
       </c>
       <c r="BJ5">
-        <v>334</v>
+        <v>664</v>
       </c>
       <c r="BK5">
-        <v>343</v>
+        <v>677</v>
       </c>
       <c r="BL5">
-        <v>345</v>
+        <v>685</v>
       </c>
       <c r="BM5">
-        <v>349</v>
+        <v>696</v>
       </c>
       <c r="BN5">
-        <v>354</v>
+        <v>703</v>
       </c>
       <c r="BO5">
-        <v>360</v>
+        <v>712</v>
       </c>
       <c r="BP5">
-        <v>366</v>
+        <v>721</v>
       </c>
       <c r="BQ5">
-        <v>370</v>
+        <v>730</v>
       </c>
       <c r="BR5">
-        <v>373</v>
+        <v>736</v>
       </c>
       <c r="BS5">
-        <v>373</v>
+        <v>739</v>
       </c>
       <c r="BT5">
-        <v>375</v>
+        <v>741</v>
       </c>
       <c r="BU5">
-        <v>380</v>
+        <v>748</v>
       </c>
       <c r="BV5">
-        <v>385</v>
+        <v>753</v>
       </c>
       <c r="BW5">
-        <v>393</v>
+        <v>761</v>
       </c>
       <c r="BX5">
-        <v>400</v>
+        <v>770</v>
       </c>
       <c r="BY5">
-        <v>408</v>
+        <v>781</v>
       </c>
       <c r="BZ5">
-        <v>418</v>
+        <v>791</v>
       </c>
     </row>
     <row r="6" spans="1:78" x14ac:dyDescent="0.25">
@@ -1624,232 +1624,232 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F6">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="G6">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="H6">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="I6">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="J6">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="K6">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="L6">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="M6">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="N6">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="O6">
-        <v>35</v>
+        <v>74</v>
       </c>
       <c r="P6">
-        <v>37</v>
+        <v>78</v>
       </c>
       <c r="Q6">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="R6">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="S6">
-        <v>47</v>
+        <v>103</v>
       </c>
       <c r="T6">
-        <v>48</v>
+        <v>106</v>
       </c>
       <c r="U6">
-        <v>49</v>
+        <v>112</v>
       </c>
       <c r="V6">
-        <v>51</v>
+        <v>115</v>
       </c>
       <c r="W6">
-        <v>53</v>
+        <v>118</v>
       </c>
       <c r="X6">
-        <v>55</v>
+        <v>122</v>
       </c>
       <c r="Y6">
-        <v>58</v>
+        <v>127</v>
       </c>
       <c r="Z6">
-        <v>60</v>
+        <v>131</v>
       </c>
       <c r="AA6">
-        <v>62</v>
+        <v>133</v>
       </c>
       <c r="AB6">
-        <v>62</v>
+        <v>136</v>
       </c>
       <c r="AC6">
-        <v>66</v>
+        <v>144</v>
       </c>
       <c r="AD6">
-        <v>66</v>
+        <v>150</v>
       </c>
       <c r="AE6">
-        <v>69</v>
+        <v>158</v>
       </c>
       <c r="AF6">
-        <v>71</v>
+        <v>166</v>
       </c>
       <c r="AG6">
-        <v>73</v>
+        <v>171</v>
       </c>
       <c r="AH6">
-        <v>75</v>
+        <v>176</v>
       </c>
       <c r="AI6">
-        <v>78</v>
+        <v>181</v>
       </c>
       <c r="AJ6">
-        <v>79</v>
+        <v>182</v>
       </c>
       <c r="AK6">
-        <v>80</v>
+        <v>186</v>
       </c>
       <c r="AL6">
-        <v>84</v>
+        <v>193</v>
       </c>
       <c r="AM6">
-        <v>89</v>
+        <v>201</v>
       </c>
       <c r="AN6">
-        <v>90</v>
+        <v>206</v>
       </c>
       <c r="AO6">
-        <v>92</v>
+        <v>211</v>
       </c>
       <c r="AP6">
-        <v>101</v>
+        <v>224</v>
       </c>
       <c r="AQ6">
-        <v>104</v>
+        <v>232</v>
       </c>
       <c r="AR6">
-        <v>105</v>
+        <v>236</v>
       </c>
       <c r="AS6">
-        <v>106</v>
+        <v>241</v>
       </c>
       <c r="AT6">
-        <v>107</v>
+        <v>249</v>
       </c>
       <c r="AU6">
-        <v>110</v>
+        <v>257</v>
       </c>
       <c r="AV6">
-        <v>110</v>
+        <v>265</v>
       </c>
       <c r="AW6">
-        <v>111</v>
+        <v>273</v>
       </c>
       <c r="AX6">
-        <v>112</v>
+        <v>281</v>
       </c>
       <c r="AY6">
-        <v>114</v>
+        <v>292</v>
       </c>
       <c r="AZ6">
-        <v>115</v>
+        <v>294</v>
       </c>
       <c r="BA6">
-        <v>116</v>
+        <v>297</v>
       </c>
       <c r="BB6">
-        <v>119</v>
+        <v>301</v>
       </c>
       <c r="BC6">
-        <v>122</v>
+        <v>308</v>
       </c>
       <c r="BD6">
-        <v>126</v>
+        <v>322</v>
       </c>
       <c r="BE6">
-        <v>129</v>
+        <v>329</v>
       </c>
       <c r="BF6">
-        <v>135</v>
+        <v>339</v>
       </c>
       <c r="BG6">
-        <v>140</v>
+        <v>347</v>
       </c>
       <c r="BH6">
-        <v>144</v>
+        <v>352</v>
       </c>
       <c r="BI6">
-        <v>148</v>
+        <v>358</v>
       </c>
       <c r="BJ6">
-        <v>149</v>
+        <v>364</v>
       </c>
       <c r="BK6">
-        <v>151</v>
+        <v>368</v>
       </c>
       <c r="BL6">
-        <v>153</v>
+        <v>374</v>
       </c>
       <c r="BM6">
-        <v>154</v>
+        <v>381</v>
       </c>
       <c r="BN6">
-        <v>157</v>
+        <v>386</v>
       </c>
       <c r="BO6">
-        <v>159</v>
+        <v>389</v>
       </c>
       <c r="BP6">
-        <v>163</v>
+        <v>393</v>
       </c>
       <c r="BQ6">
-        <v>163</v>
+        <v>395</v>
       </c>
       <c r="BR6">
-        <v>167</v>
+        <v>402</v>
       </c>
       <c r="BS6">
-        <v>170</v>
+        <v>408</v>
       </c>
       <c r="BT6">
-        <v>171</v>
+        <v>410</v>
       </c>
       <c r="BU6">
-        <v>175</v>
+        <v>418</v>
       </c>
       <c r="BV6">
-        <v>177</v>
+        <v>421</v>
       </c>
       <c r="BW6">
-        <v>181</v>
+        <v>429</v>
       </c>
       <c r="BX6">
-        <v>184</v>
+        <v>437</v>
       </c>
       <c r="BY6">
-        <v>186</v>
+        <v>443</v>
       </c>
       <c r="BZ6">
-        <v>187</v>
+        <v>446</v>
       </c>
     </row>
     <row r="7" spans="1:78" x14ac:dyDescent="0.25">
@@ -1860,232 +1860,232 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="F7">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="G7">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="H7">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="I7">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="J7">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="K7">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="L7">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="M7">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="N7">
-        <v>23</v>
+        <v>96</v>
       </c>
       <c r="O7">
-        <v>25</v>
+        <v>110</v>
       </c>
       <c r="P7">
-        <v>26</v>
+        <v>118</v>
       </c>
       <c r="Q7">
-        <v>28</v>
+        <v>129</v>
       </c>
       <c r="R7">
-        <v>29</v>
+        <v>135</v>
       </c>
       <c r="S7">
-        <v>32</v>
+        <v>141</v>
       </c>
       <c r="T7">
-        <v>34</v>
+        <v>154</v>
       </c>
       <c r="U7">
-        <v>34</v>
+        <v>162</v>
       </c>
       <c r="V7">
-        <v>35</v>
+        <v>178</v>
       </c>
       <c r="W7">
-        <v>35</v>
+        <v>183</v>
       </c>
       <c r="X7">
-        <v>39</v>
+        <v>195</v>
       </c>
       <c r="Y7">
-        <v>41</v>
+        <v>204</v>
       </c>
       <c r="Z7">
-        <v>41</v>
+        <v>211</v>
       </c>
       <c r="AA7">
-        <v>43</v>
+        <v>222</v>
       </c>
       <c r="AB7">
-        <v>43</v>
+        <v>224</v>
       </c>
       <c r="AC7">
-        <v>45</v>
+        <v>234</v>
       </c>
       <c r="AD7">
-        <v>46</v>
+        <v>243</v>
       </c>
       <c r="AE7">
-        <v>48</v>
+        <v>252</v>
       </c>
       <c r="AF7">
-        <v>49</v>
+        <v>264</v>
       </c>
       <c r="AG7">
-        <v>50</v>
+        <v>277</v>
       </c>
       <c r="AH7">
-        <v>51</v>
+        <v>287</v>
       </c>
       <c r="AI7">
-        <v>51</v>
+        <v>292</v>
       </c>
       <c r="AJ7">
-        <v>51</v>
+        <v>300</v>
       </c>
       <c r="AK7">
-        <v>53</v>
+        <v>310</v>
       </c>
       <c r="AL7">
-        <v>57</v>
+        <v>316</v>
       </c>
       <c r="AM7">
-        <v>57</v>
+        <v>322</v>
       </c>
       <c r="AN7">
-        <v>57</v>
+        <v>324</v>
       </c>
       <c r="AO7">
-        <v>57</v>
+        <v>329</v>
       </c>
       <c r="AP7">
-        <v>58</v>
+        <v>335</v>
       </c>
       <c r="AQ7">
-        <v>62</v>
+        <v>344</v>
       </c>
       <c r="AR7">
-        <v>64</v>
+        <v>348</v>
       </c>
       <c r="AS7">
-        <v>65</v>
+        <v>351</v>
       </c>
       <c r="AT7">
-        <v>65</v>
+        <v>356</v>
       </c>
       <c r="AU7">
-        <v>66</v>
+        <v>367</v>
       </c>
       <c r="AV7">
-        <v>68</v>
+        <v>374</v>
       </c>
       <c r="AW7">
-        <v>69</v>
+        <v>384</v>
       </c>
       <c r="AX7">
-        <v>73</v>
+        <v>402</v>
       </c>
       <c r="AY7">
-        <v>74</v>
+        <v>407</v>
       </c>
       <c r="AZ7">
-        <v>74</v>
+        <v>411</v>
       </c>
       <c r="BA7">
-        <v>74</v>
+        <v>418</v>
       </c>
       <c r="BB7">
-        <v>74</v>
+        <v>422</v>
       </c>
       <c r="BC7">
-        <v>77</v>
+        <v>431</v>
       </c>
       <c r="BD7">
-        <v>78</v>
+        <v>439</v>
       </c>
       <c r="BE7">
-        <v>81</v>
+        <v>453</v>
       </c>
       <c r="BF7">
-        <v>82</v>
+        <v>458</v>
       </c>
       <c r="BG7">
-        <v>84</v>
+        <v>463</v>
       </c>
       <c r="BH7">
-        <v>87</v>
+        <v>472</v>
       </c>
       <c r="BI7">
-        <v>87</v>
+        <v>477</v>
       </c>
       <c r="BJ7">
-        <v>90</v>
+        <v>489</v>
       </c>
       <c r="BK7">
-        <v>93</v>
+        <v>492</v>
       </c>
       <c r="BL7">
-        <v>95</v>
+        <v>507</v>
       </c>
       <c r="BM7">
-        <v>95</v>
+        <v>518</v>
       </c>
       <c r="BN7">
-        <v>98</v>
+        <v>532</v>
       </c>
       <c r="BO7">
-        <v>99</v>
+        <v>538</v>
       </c>
       <c r="BP7">
-        <v>101</v>
+        <v>545</v>
       </c>
       <c r="BQ7">
-        <v>104</v>
+        <v>551</v>
       </c>
       <c r="BR7">
-        <v>109</v>
+        <v>559</v>
       </c>
       <c r="BS7">
-        <v>112</v>
+        <v>565</v>
       </c>
       <c r="BT7">
-        <v>113</v>
+        <v>566</v>
       </c>
       <c r="BU7">
-        <v>120</v>
+        <v>576</v>
       </c>
       <c r="BV7">
-        <v>123</v>
+        <v>583</v>
       </c>
       <c r="BW7">
-        <v>125</v>
+        <v>589</v>
       </c>
       <c r="BX7">
-        <v>126</v>
+        <v>593</v>
       </c>
       <c r="BY7">
-        <v>128</v>
+        <v>597</v>
       </c>
       <c r="BZ7">
-        <v>129</v>
+        <v>600</v>
       </c>
     </row>
     <row r="8" spans="1:78" x14ac:dyDescent="0.25">
@@ -2096,232 +2096,232 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D8">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E8">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="F8">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="G8">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="H8">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="I8">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="J8">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="K8">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="L8">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="M8">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="N8">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="O8">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="P8">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="Q8">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="R8">
-        <v>33</v>
+        <v>83</v>
       </c>
       <c r="S8">
-        <v>35</v>
+        <v>89</v>
       </c>
       <c r="T8">
-        <v>36</v>
+        <v>94</v>
       </c>
       <c r="U8">
-        <v>36</v>
+        <v>97</v>
       </c>
       <c r="V8">
-        <v>41</v>
+        <v>108</v>
       </c>
       <c r="W8">
-        <v>41</v>
+        <v>114</v>
       </c>
       <c r="X8">
-        <v>42</v>
+        <v>119</v>
       </c>
       <c r="Y8">
-        <v>43</v>
+        <v>122</v>
       </c>
       <c r="Z8">
-        <v>44</v>
+        <v>123</v>
       </c>
       <c r="AA8">
-        <v>44</v>
+        <v>127</v>
       </c>
       <c r="AB8">
-        <v>46</v>
+        <v>130</v>
       </c>
       <c r="AC8">
-        <v>49</v>
+        <v>133</v>
       </c>
       <c r="AD8">
-        <v>50</v>
+        <v>137</v>
       </c>
       <c r="AE8">
-        <v>53</v>
+        <v>144</v>
       </c>
       <c r="AF8">
-        <v>55</v>
+        <v>150</v>
       </c>
       <c r="AG8">
-        <v>56</v>
+        <v>154</v>
       </c>
       <c r="AH8">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="AI8">
-        <v>62</v>
+        <v>167</v>
       </c>
       <c r="AJ8">
-        <v>63</v>
+        <v>178</v>
       </c>
       <c r="AK8">
-        <v>64</v>
+        <v>183</v>
       </c>
       <c r="AL8">
-        <v>64</v>
+        <v>186</v>
       </c>
       <c r="AM8">
-        <v>64</v>
+        <v>186</v>
       </c>
       <c r="AN8">
-        <v>64</v>
+        <v>189</v>
       </c>
       <c r="AO8">
-        <v>65</v>
+        <v>199</v>
       </c>
       <c r="AP8">
-        <v>66</v>
+        <v>206</v>
       </c>
       <c r="AQ8">
-        <v>69</v>
+        <v>214</v>
       </c>
       <c r="AR8">
-        <v>69</v>
+        <v>219</v>
       </c>
       <c r="AS8">
-        <v>69</v>
+        <v>225</v>
       </c>
       <c r="AT8">
-        <v>72</v>
+        <v>231</v>
       </c>
       <c r="AU8">
-        <v>72</v>
+        <v>232</v>
       </c>
       <c r="AV8">
-        <v>75</v>
+        <v>237</v>
       </c>
       <c r="AW8">
-        <v>76</v>
+        <v>242</v>
       </c>
       <c r="AX8">
-        <v>76</v>
+        <v>245</v>
       </c>
       <c r="AY8">
-        <v>76</v>
+        <v>249</v>
       </c>
       <c r="AZ8">
-        <v>77</v>
+        <v>256</v>
       </c>
       <c r="BA8">
-        <v>78</v>
+        <v>258</v>
       </c>
       <c r="BB8">
-        <v>79</v>
+        <v>259</v>
       </c>
       <c r="BC8">
-        <v>81</v>
+        <v>265</v>
       </c>
       <c r="BD8">
-        <v>84</v>
+        <v>272</v>
       </c>
       <c r="BE8">
-        <v>85</v>
+        <v>280</v>
       </c>
       <c r="BF8">
-        <v>87</v>
+        <v>286</v>
       </c>
       <c r="BG8">
-        <v>89</v>
+        <v>289</v>
       </c>
       <c r="BH8">
-        <v>92</v>
+        <v>293</v>
       </c>
       <c r="BI8">
-        <v>94</v>
+        <v>301</v>
       </c>
       <c r="BJ8">
-        <v>96</v>
+        <v>305</v>
       </c>
       <c r="BK8">
-        <v>98</v>
+        <v>315</v>
       </c>
       <c r="BL8">
-        <v>101</v>
+        <v>318</v>
       </c>
       <c r="BM8">
-        <v>103</v>
+        <v>323</v>
       </c>
       <c r="BN8">
-        <v>106</v>
+        <v>326</v>
       </c>
       <c r="BO8">
-        <v>106</v>
+        <v>328</v>
       </c>
       <c r="BP8">
-        <v>107</v>
+        <v>333</v>
       </c>
       <c r="BQ8">
-        <v>110</v>
+        <v>338</v>
       </c>
       <c r="BR8">
-        <v>110</v>
+        <v>338</v>
       </c>
       <c r="BS8">
-        <v>110</v>
+        <v>339</v>
       </c>
       <c r="BT8">
-        <v>110</v>
+        <v>340</v>
       </c>
       <c r="BU8">
-        <v>110</v>
+        <v>343</v>
       </c>
       <c r="BV8">
-        <v>110</v>
+        <v>344</v>
       </c>
       <c r="BW8">
-        <v>110</v>
+        <v>344</v>
       </c>
       <c r="BX8">
-        <v>110</v>
+        <v>346</v>
       </c>
       <c r="BY8">
-        <v>113</v>
+        <v>349</v>
       </c>
       <c r="BZ8">
-        <v>115</v>
+        <v>353</v>
       </c>
     </row>
     <row r="9" spans="1:78" x14ac:dyDescent="0.25">
@@ -2332,232 +2332,232 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D9">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E9">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="F9">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="G9">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="H9">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="I9">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="J9">
-        <v>34</v>
+        <v>86</v>
       </c>
       <c r="K9">
-        <v>36</v>
+        <v>96</v>
       </c>
       <c r="L9">
-        <v>37</v>
+        <v>99</v>
       </c>
       <c r="M9">
-        <v>41</v>
+        <v>105</v>
       </c>
       <c r="N9">
-        <v>46</v>
+        <v>121</v>
       </c>
       <c r="O9">
-        <v>49</v>
+        <v>134</v>
       </c>
       <c r="P9">
-        <v>50</v>
+        <v>139</v>
       </c>
       <c r="Q9">
-        <v>51</v>
+        <v>145</v>
       </c>
       <c r="R9">
-        <v>58</v>
+        <v>161</v>
       </c>
       <c r="S9">
-        <v>64</v>
+        <v>171</v>
       </c>
       <c r="T9">
-        <v>65</v>
+        <v>180</v>
       </c>
       <c r="U9">
-        <v>67</v>
+        <v>193</v>
       </c>
       <c r="V9">
-        <v>67</v>
+        <v>204</v>
       </c>
       <c r="W9">
-        <v>72</v>
+        <v>216</v>
       </c>
       <c r="X9">
-        <v>80</v>
+        <v>230</v>
       </c>
       <c r="Y9">
-        <v>84</v>
+        <v>242</v>
       </c>
       <c r="Z9">
-        <v>84</v>
+        <v>254</v>
       </c>
       <c r="AA9">
-        <v>87</v>
+        <v>265</v>
       </c>
       <c r="AB9">
-        <v>87</v>
+        <v>271</v>
       </c>
       <c r="AC9">
-        <v>89</v>
+        <v>279</v>
       </c>
       <c r="AD9">
-        <v>91</v>
+        <v>288</v>
       </c>
       <c r="AE9">
-        <v>95</v>
+        <v>298</v>
       </c>
       <c r="AF9">
-        <v>101</v>
+        <v>311</v>
       </c>
       <c r="AG9">
-        <v>105</v>
+        <v>320</v>
       </c>
       <c r="AH9">
-        <v>109</v>
+        <v>329</v>
       </c>
       <c r="AI9">
-        <v>111</v>
+        <v>335</v>
       </c>
       <c r="AJ9">
-        <v>114</v>
+        <v>341</v>
       </c>
       <c r="AK9">
-        <v>117</v>
+        <v>354</v>
       </c>
       <c r="AL9">
-        <v>118</v>
+        <v>357</v>
       </c>
       <c r="AM9">
-        <v>119</v>
+        <v>364</v>
       </c>
       <c r="AN9">
-        <v>119</v>
+        <v>371</v>
       </c>
       <c r="AO9">
-        <v>121</v>
+        <v>379</v>
       </c>
       <c r="AP9">
-        <v>121</v>
+        <v>389</v>
       </c>
       <c r="AQ9">
-        <v>124</v>
+        <v>395</v>
       </c>
       <c r="AR9">
-        <v>127</v>
+        <v>411</v>
       </c>
       <c r="AS9">
-        <v>129</v>
+        <v>420</v>
       </c>
       <c r="AT9">
-        <v>130</v>
+        <v>429</v>
       </c>
       <c r="AU9">
-        <v>133</v>
+        <v>439</v>
       </c>
       <c r="AV9">
-        <v>136</v>
+        <v>449</v>
       </c>
       <c r="AW9">
-        <v>138</v>
+        <v>457</v>
       </c>
       <c r="AX9">
-        <v>140</v>
+        <v>469</v>
       </c>
       <c r="AY9">
-        <v>143</v>
+        <v>481</v>
       </c>
       <c r="AZ9">
-        <v>143</v>
+        <v>489</v>
       </c>
       <c r="BA9">
-        <v>144</v>
+        <v>499</v>
       </c>
       <c r="BB9">
-        <v>145</v>
+        <v>505</v>
       </c>
       <c r="BC9">
-        <v>149</v>
+        <v>517</v>
       </c>
       <c r="BD9">
-        <v>153</v>
+        <v>529</v>
       </c>
       <c r="BE9">
-        <v>155</v>
+        <v>541</v>
       </c>
       <c r="BF9">
-        <v>159</v>
+        <v>550</v>
       </c>
       <c r="BG9">
-        <v>162</v>
+        <v>557</v>
       </c>
       <c r="BH9">
-        <v>164</v>
+        <v>561</v>
       </c>
       <c r="BI9">
-        <v>165</v>
+        <v>563</v>
       </c>
       <c r="BJ9">
-        <v>167</v>
+        <v>569</v>
       </c>
       <c r="BK9">
-        <v>171</v>
+        <v>582</v>
       </c>
       <c r="BL9">
-        <v>173</v>
+        <v>592</v>
       </c>
       <c r="BM9">
-        <v>175</v>
+        <v>603</v>
       </c>
       <c r="BN9">
-        <v>177</v>
+        <v>607</v>
       </c>
       <c r="BO9">
-        <v>180</v>
+        <v>615</v>
       </c>
       <c r="BP9">
-        <v>184</v>
+        <v>622</v>
       </c>
       <c r="BQ9">
-        <v>186</v>
+        <v>627</v>
       </c>
       <c r="BR9">
-        <v>188</v>
+        <v>631</v>
       </c>
       <c r="BS9">
-        <v>190</v>
+        <v>638</v>
       </c>
       <c r="BT9">
-        <v>190</v>
+        <v>639</v>
       </c>
       <c r="BU9">
-        <v>191</v>
+        <v>642</v>
       </c>
       <c r="BV9">
-        <v>191</v>
+        <v>644</v>
       </c>
       <c r="BW9">
-        <v>195</v>
+        <v>650</v>
       </c>
       <c r="BX9">
-        <v>198</v>
+        <v>656</v>
       </c>
       <c r="BY9">
-        <v>200</v>
+        <v>665</v>
       </c>
       <c r="BZ9">
-        <v>200</v>
+        <v>665</v>
       </c>
     </row>
     <row r="10" spans="1:78" x14ac:dyDescent="0.25">
@@ -2568,232 +2568,232 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E10">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="F10">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="G10">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="H10">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="I10">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="J10">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="K10">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="L10">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="M10">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="N10">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="O10">
-        <v>20</v>
+        <v>98</v>
       </c>
       <c r="P10">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="Q10">
-        <v>27</v>
+        <v>114</v>
       </c>
       <c r="R10">
-        <v>29</v>
+        <v>123</v>
       </c>
       <c r="S10">
-        <v>31</v>
+        <v>128</v>
       </c>
       <c r="T10">
-        <v>35</v>
+        <v>138</v>
       </c>
       <c r="U10">
-        <v>37</v>
+        <v>144</v>
       </c>
       <c r="V10">
-        <v>38</v>
+        <v>153</v>
       </c>
       <c r="W10">
-        <v>39</v>
+        <v>163</v>
       </c>
       <c r="X10">
-        <v>41</v>
+        <v>172</v>
       </c>
       <c r="Y10">
-        <v>42</v>
+        <v>181</v>
       </c>
       <c r="Z10">
-        <v>42</v>
+        <v>188</v>
       </c>
       <c r="AA10">
-        <v>44</v>
+        <v>192</v>
       </c>
       <c r="AB10">
-        <v>44</v>
+        <v>200</v>
       </c>
       <c r="AC10">
-        <v>45</v>
+        <v>206</v>
       </c>
       <c r="AD10">
-        <v>46</v>
+        <v>214</v>
       </c>
       <c r="AE10">
-        <v>48</v>
+        <v>222</v>
       </c>
       <c r="AF10">
-        <v>50</v>
+        <v>228</v>
       </c>
       <c r="AG10">
-        <v>50</v>
+        <v>235</v>
       </c>
       <c r="AH10">
-        <v>54</v>
+        <v>245</v>
       </c>
       <c r="AI10">
-        <v>54</v>
+        <v>246</v>
       </c>
       <c r="AJ10">
-        <v>54</v>
+        <v>253</v>
       </c>
       <c r="AK10">
-        <v>55</v>
+        <v>257</v>
       </c>
       <c r="AL10">
-        <v>55</v>
+        <v>262</v>
       </c>
       <c r="AM10">
-        <v>57</v>
+        <v>270</v>
       </c>
       <c r="AN10">
-        <v>57</v>
+        <v>273</v>
       </c>
       <c r="AO10">
-        <v>59</v>
+        <v>280</v>
       </c>
       <c r="AP10">
-        <v>64</v>
+        <v>286</v>
       </c>
       <c r="AQ10">
-        <v>68</v>
+        <v>295</v>
       </c>
       <c r="AR10">
-        <v>71</v>
+        <v>303</v>
       </c>
       <c r="AS10">
-        <v>72</v>
+        <v>309</v>
       </c>
       <c r="AT10">
-        <v>73</v>
+        <v>314</v>
       </c>
       <c r="AU10">
-        <v>74</v>
+        <v>318</v>
       </c>
       <c r="AV10">
-        <v>74</v>
+        <v>326</v>
       </c>
       <c r="AW10">
-        <v>74</v>
+        <v>330</v>
       </c>
       <c r="AX10">
-        <v>78</v>
+        <v>341</v>
       </c>
       <c r="AY10">
-        <v>79</v>
+        <v>350</v>
       </c>
       <c r="AZ10">
-        <v>79</v>
+        <v>354</v>
       </c>
       <c r="BA10">
-        <v>82</v>
+        <v>360</v>
       </c>
       <c r="BB10">
-        <v>82</v>
+        <v>363</v>
       </c>
       <c r="BC10">
-        <v>83</v>
+        <v>365</v>
       </c>
       <c r="BD10">
-        <v>84</v>
+        <v>371</v>
       </c>
       <c r="BE10">
-        <v>85</v>
+        <v>376</v>
       </c>
       <c r="BF10">
-        <v>88</v>
+        <v>384</v>
       </c>
       <c r="BG10">
-        <v>90</v>
+        <v>389</v>
       </c>
       <c r="BH10">
-        <v>94</v>
+        <v>394</v>
       </c>
       <c r="BI10">
-        <v>94</v>
+        <v>397</v>
       </c>
       <c r="BJ10">
-        <v>95</v>
+        <v>401</v>
       </c>
       <c r="BK10">
-        <v>95</v>
+        <v>405</v>
       </c>
       <c r="BL10">
-        <v>97</v>
+        <v>409</v>
       </c>
       <c r="BM10">
-        <v>97</v>
+        <v>413</v>
       </c>
       <c r="BN10">
-        <v>100</v>
+        <v>419</v>
       </c>
       <c r="BO10">
-        <v>100</v>
+        <v>423</v>
       </c>
       <c r="BP10">
-        <v>101</v>
+        <v>427</v>
       </c>
       <c r="BQ10">
-        <v>101</v>
+        <v>436</v>
       </c>
       <c r="BR10">
-        <v>102</v>
+        <v>440</v>
       </c>
       <c r="BS10">
-        <v>102</v>
+        <v>443</v>
       </c>
       <c r="BT10">
-        <v>102</v>
+        <v>444</v>
       </c>
       <c r="BU10">
-        <v>102</v>
+        <v>445</v>
       </c>
       <c r="BV10">
-        <v>103</v>
+        <v>446</v>
       </c>
       <c r="BW10">
-        <v>103</v>
+        <v>448</v>
       </c>
       <c r="BX10">
-        <v>104</v>
+        <v>452</v>
       </c>
       <c r="BY10">
-        <v>105</v>
+        <v>454</v>
       </c>
       <c r="BZ10">
-        <v>106</v>
+        <v>455</v>
       </c>
     </row>
     <row r="11" spans="1:78" x14ac:dyDescent="0.25">
@@ -2804,232 +2804,232 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D11">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="E11">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="F11">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G11">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="H11">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="I11">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="J11">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="K11">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="L11">
-        <v>27</v>
+        <v>84</v>
       </c>
       <c r="M11">
-        <v>32</v>
+        <v>93</v>
       </c>
       <c r="N11">
-        <v>34</v>
+        <v>100</v>
       </c>
       <c r="O11">
-        <v>35</v>
+        <v>105</v>
       </c>
       <c r="P11">
-        <v>35</v>
+        <v>107</v>
       </c>
       <c r="Q11">
-        <v>40</v>
+        <v>113</v>
       </c>
       <c r="R11">
-        <v>40</v>
+        <v>117</v>
       </c>
       <c r="S11">
-        <v>41</v>
+        <v>118</v>
       </c>
       <c r="T11">
-        <v>44</v>
+        <v>122</v>
       </c>
       <c r="U11">
-        <v>52</v>
+        <v>134</v>
       </c>
       <c r="V11">
-        <v>52</v>
+        <v>140</v>
       </c>
       <c r="W11">
-        <v>55</v>
+        <v>150</v>
       </c>
       <c r="X11">
-        <v>60</v>
+        <v>162</v>
       </c>
       <c r="Y11">
-        <v>64</v>
+        <v>170</v>
       </c>
       <c r="Z11">
-        <v>71</v>
+        <v>179</v>
       </c>
       <c r="AA11">
-        <v>73</v>
+        <v>186</v>
       </c>
       <c r="AB11">
-        <v>76</v>
+        <v>189</v>
       </c>
       <c r="AC11">
-        <v>77</v>
+        <v>193</v>
       </c>
       <c r="AD11">
-        <v>79</v>
+        <v>196</v>
       </c>
       <c r="AE11">
-        <v>81</v>
+        <v>203</v>
       </c>
       <c r="AF11">
-        <v>85</v>
+        <v>214</v>
       </c>
       <c r="AG11">
-        <v>88</v>
+        <v>221</v>
       </c>
       <c r="AH11">
-        <v>93</v>
+        <v>227</v>
       </c>
       <c r="AI11">
-        <v>101</v>
+        <v>239</v>
       </c>
       <c r="AJ11">
-        <v>104</v>
+        <v>247</v>
       </c>
       <c r="AK11">
-        <v>105</v>
+        <v>249</v>
       </c>
       <c r="AL11">
-        <v>108</v>
+        <v>257</v>
       </c>
       <c r="AM11">
-        <v>112</v>
+        <v>264</v>
       </c>
       <c r="AN11">
-        <v>114</v>
+        <v>267</v>
       </c>
       <c r="AO11">
-        <v>122</v>
+        <v>278</v>
       </c>
       <c r="AP11">
-        <v>127</v>
+        <v>288</v>
       </c>
       <c r="AQ11">
-        <v>129</v>
+        <v>298</v>
       </c>
       <c r="AR11">
-        <v>130</v>
+        <v>302</v>
       </c>
       <c r="AS11">
-        <v>132</v>
+        <v>309</v>
       </c>
       <c r="AT11">
-        <v>132</v>
+        <v>316</v>
       </c>
       <c r="AU11">
-        <v>134</v>
+        <v>322</v>
       </c>
       <c r="AV11">
-        <v>136</v>
+        <v>330</v>
       </c>
       <c r="AW11">
-        <v>138</v>
+        <v>339</v>
       </c>
       <c r="AX11">
-        <v>141</v>
+        <v>346</v>
       </c>
       <c r="AY11">
-        <v>145</v>
+        <v>355</v>
       </c>
       <c r="AZ11">
-        <v>146</v>
+        <v>360</v>
       </c>
       <c r="BA11">
-        <v>148</v>
+        <v>363</v>
       </c>
       <c r="BB11">
-        <v>151</v>
+        <v>368</v>
       </c>
       <c r="BC11">
-        <v>153</v>
+        <v>374</v>
       </c>
       <c r="BD11">
-        <v>155</v>
+        <v>383</v>
       </c>
       <c r="BE11">
-        <v>165</v>
+        <v>398</v>
       </c>
       <c r="BF11">
-        <v>172</v>
+        <v>415</v>
       </c>
       <c r="BG11">
-        <v>177</v>
+        <v>421</v>
       </c>
       <c r="BH11">
-        <v>178</v>
+        <v>424</v>
       </c>
       <c r="BI11">
-        <v>181</v>
+        <v>429</v>
       </c>
       <c r="BJ11">
-        <v>186</v>
+        <v>437</v>
       </c>
       <c r="BK11">
-        <v>190</v>
+        <v>444</v>
       </c>
       <c r="BL11">
-        <v>192</v>
+        <v>449</v>
       </c>
       <c r="BM11">
-        <v>194</v>
+        <v>457</v>
       </c>
       <c r="BN11">
-        <v>194</v>
+        <v>460</v>
       </c>
       <c r="BO11">
-        <v>194</v>
+        <v>463</v>
       </c>
       <c r="BP11">
-        <v>197</v>
+        <v>469</v>
       </c>
       <c r="BQ11">
-        <v>200</v>
+        <v>474</v>
       </c>
       <c r="BR11">
-        <v>204</v>
+        <v>478</v>
       </c>
       <c r="BS11">
-        <v>207</v>
+        <v>483</v>
       </c>
       <c r="BT11">
-        <v>207</v>
+        <v>483</v>
       </c>
       <c r="BU11">
-        <v>209</v>
+        <v>488</v>
       </c>
       <c r="BV11">
-        <v>209</v>
+        <v>488</v>
       </c>
       <c r="BW11">
-        <v>212</v>
+        <v>495</v>
       </c>
       <c r="BX11">
-        <v>213</v>
+        <v>499</v>
       </c>
       <c r="BY11">
-        <v>214</v>
+        <v>500</v>
       </c>
       <c r="BZ11">
-        <v>218</v>
+        <v>505</v>
       </c>
     </row>
     <row r="12" spans="1:78" x14ac:dyDescent="0.25">
@@ -3040,232 +3040,232 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E12">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="F12">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="G12">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="H12">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="I12">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="J12">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="K12">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="L12">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="M12">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="N12">
-        <v>39</v>
+        <v>103</v>
       </c>
       <c r="O12">
-        <v>39</v>
+        <v>107</v>
       </c>
       <c r="P12">
-        <v>41</v>
+        <v>114</v>
       </c>
       <c r="Q12">
-        <v>44</v>
+        <v>121</v>
       </c>
       <c r="R12">
-        <v>46</v>
+        <v>131</v>
       </c>
       <c r="S12">
-        <v>55</v>
+        <v>142</v>
       </c>
       <c r="T12">
-        <v>55</v>
+        <v>145</v>
       </c>
       <c r="U12">
-        <v>56</v>
+        <v>149</v>
       </c>
       <c r="V12">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="W12">
-        <v>62</v>
+        <v>159</v>
       </c>
       <c r="X12">
-        <v>65</v>
+        <v>166</v>
       </c>
       <c r="Y12">
-        <v>68</v>
+        <v>174</v>
       </c>
       <c r="Z12">
-        <v>68</v>
+        <v>178</v>
       </c>
       <c r="AA12">
-        <v>69</v>
+        <v>182</v>
       </c>
       <c r="AB12">
-        <v>74</v>
+        <v>190</v>
       </c>
       <c r="AC12">
-        <v>75</v>
+        <v>194</v>
       </c>
       <c r="AD12">
-        <v>76</v>
+        <v>199</v>
       </c>
       <c r="AE12">
-        <v>82</v>
+        <v>215</v>
       </c>
       <c r="AF12">
-        <v>82</v>
+        <v>218</v>
       </c>
       <c r="AG12">
-        <v>87</v>
+        <v>226</v>
       </c>
       <c r="AH12">
-        <v>90</v>
+        <v>232</v>
       </c>
       <c r="AI12">
-        <v>99</v>
+        <v>244</v>
       </c>
       <c r="AJ12">
-        <v>104</v>
+        <v>254</v>
       </c>
       <c r="AK12">
-        <v>107</v>
+        <v>261</v>
       </c>
       <c r="AL12">
-        <v>110</v>
+        <v>269</v>
       </c>
       <c r="AM12">
-        <v>112</v>
+        <v>276</v>
       </c>
       <c r="AN12">
-        <v>115</v>
+        <v>286</v>
       </c>
       <c r="AO12">
-        <v>117</v>
+        <v>292</v>
       </c>
       <c r="AP12">
-        <v>119</v>
+        <v>296</v>
       </c>
       <c r="AQ12">
-        <v>122</v>
+        <v>307</v>
       </c>
       <c r="AR12">
-        <v>126</v>
+        <v>316</v>
       </c>
       <c r="AS12">
-        <v>129</v>
+        <v>324</v>
       </c>
       <c r="AT12">
-        <v>132</v>
+        <v>332</v>
       </c>
       <c r="AU12">
-        <v>134</v>
+        <v>337</v>
       </c>
       <c r="AV12">
-        <v>138</v>
+        <v>344</v>
       </c>
       <c r="AW12">
-        <v>143</v>
+        <v>353</v>
       </c>
       <c r="AX12">
-        <v>143</v>
+        <v>359</v>
       </c>
       <c r="AY12">
-        <v>145</v>
+        <v>368</v>
       </c>
       <c r="AZ12">
-        <v>146</v>
+        <v>370</v>
       </c>
       <c r="BA12">
-        <v>147</v>
+        <v>374</v>
       </c>
       <c r="BB12">
-        <v>149</v>
+        <v>377</v>
       </c>
       <c r="BC12">
-        <v>153</v>
+        <v>382</v>
       </c>
       <c r="BD12">
-        <v>155</v>
+        <v>390</v>
       </c>
       <c r="BE12">
-        <v>157</v>
+        <v>401</v>
       </c>
       <c r="BF12">
-        <v>160</v>
+        <v>409</v>
       </c>
       <c r="BG12">
-        <v>161</v>
+        <v>412</v>
       </c>
       <c r="BH12">
-        <v>163</v>
+        <v>419</v>
       </c>
       <c r="BI12">
-        <v>164</v>
+        <v>422</v>
       </c>
       <c r="BJ12">
-        <v>167</v>
+        <v>429</v>
       </c>
       <c r="BK12">
-        <v>168</v>
+        <v>435</v>
       </c>
       <c r="BL12">
-        <v>171</v>
+        <v>442</v>
       </c>
       <c r="BM12">
-        <v>172</v>
+        <v>453</v>
       </c>
       <c r="BN12">
-        <v>174</v>
+        <v>459</v>
       </c>
       <c r="BO12">
-        <v>174</v>
+        <v>461</v>
       </c>
       <c r="BP12">
-        <v>177</v>
+        <v>466</v>
       </c>
       <c r="BQ12">
-        <v>180</v>
+        <v>472</v>
       </c>
       <c r="BR12">
-        <v>186</v>
+        <v>481</v>
       </c>
       <c r="BS12">
-        <v>190</v>
+        <v>486</v>
       </c>
       <c r="BT12">
-        <v>191</v>
+        <v>488</v>
       </c>
       <c r="BU12">
-        <v>195</v>
+        <v>493</v>
       </c>
       <c r="BV12">
-        <v>196</v>
+        <v>499</v>
       </c>
       <c r="BW12">
-        <v>198</v>
+        <v>504</v>
       </c>
       <c r="BX12">
-        <v>200</v>
+        <v>508</v>
       </c>
       <c r="BY12">
-        <v>205</v>
+        <v>514</v>
       </c>
       <c r="BZ12">
-        <v>207</v>
+        <v>516</v>
       </c>
     </row>
     <row r="13" spans="1:78" x14ac:dyDescent="0.25">
@@ -3276,232 +3276,232 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="E13">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F13">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="G13">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="H13">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="I13">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="J13">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="K13">
-        <v>17</v>
+        <v>104</v>
       </c>
       <c r="L13">
-        <v>20</v>
+        <v>114</v>
       </c>
       <c r="M13">
-        <v>21</v>
+        <v>122</v>
       </c>
       <c r="N13">
-        <v>28</v>
+        <v>137</v>
       </c>
       <c r="O13">
-        <v>28</v>
+        <v>146</v>
       </c>
       <c r="P13">
-        <v>31</v>
+        <v>158</v>
       </c>
       <c r="Q13">
-        <v>34</v>
+        <v>171</v>
       </c>
       <c r="R13">
-        <v>35</v>
+        <v>178</v>
       </c>
       <c r="S13">
-        <v>37</v>
+        <v>186</v>
       </c>
       <c r="T13">
-        <v>38</v>
+        <v>190</v>
       </c>
       <c r="U13">
-        <v>41</v>
+        <v>202</v>
       </c>
       <c r="V13">
-        <v>44</v>
+        <v>213</v>
       </c>
       <c r="W13">
-        <v>44</v>
+        <v>216</v>
       </c>
       <c r="X13">
-        <v>44</v>
+        <v>226</v>
       </c>
       <c r="Y13">
-        <v>44</v>
+        <v>232</v>
       </c>
       <c r="Z13">
-        <v>46</v>
+        <v>239</v>
       </c>
       <c r="AA13">
-        <v>50</v>
+        <v>254</v>
       </c>
       <c r="AB13">
-        <v>52</v>
+        <v>268</v>
       </c>
       <c r="AC13">
-        <v>52</v>
+        <v>275</v>
       </c>
       <c r="AD13">
-        <v>54</v>
+        <v>284</v>
       </c>
       <c r="AE13">
-        <v>55</v>
+        <v>297</v>
       </c>
       <c r="AF13">
-        <v>57</v>
+        <v>305</v>
       </c>
       <c r="AG13">
-        <v>61</v>
+        <v>312</v>
       </c>
       <c r="AH13">
-        <v>61</v>
+        <v>314</v>
       </c>
       <c r="AI13">
-        <v>62</v>
+        <v>320</v>
       </c>
       <c r="AJ13">
-        <v>65</v>
+        <v>325</v>
       </c>
       <c r="AK13">
-        <v>68</v>
+        <v>332</v>
       </c>
       <c r="AL13">
-        <v>68</v>
+        <v>336</v>
       </c>
       <c r="AM13">
-        <v>68</v>
+        <v>344</v>
       </c>
       <c r="AN13">
-        <v>70</v>
+        <v>351</v>
       </c>
       <c r="AO13">
-        <v>72</v>
+        <v>357</v>
       </c>
       <c r="AP13">
-        <v>74</v>
+        <v>365</v>
       </c>
       <c r="AQ13">
-        <v>83</v>
+        <v>380</v>
       </c>
       <c r="AR13">
-        <v>85</v>
+        <v>390</v>
       </c>
       <c r="AS13">
-        <v>87</v>
+        <v>403</v>
       </c>
       <c r="AT13">
-        <v>88</v>
+        <v>418</v>
       </c>
       <c r="AU13">
-        <v>90</v>
+        <v>428</v>
       </c>
       <c r="AV13">
-        <v>98</v>
+        <v>449</v>
       </c>
       <c r="AW13">
-        <v>101</v>
+        <v>462</v>
       </c>
       <c r="AX13">
-        <v>103</v>
+        <v>472</v>
       </c>
       <c r="AY13">
-        <v>104</v>
+        <v>480</v>
       </c>
       <c r="AZ13">
-        <v>105</v>
+        <v>487</v>
       </c>
       <c r="BA13">
-        <v>107</v>
+        <v>498</v>
       </c>
       <c r="BB13">
-        <v>108</v>
+        <v>506</v>
       </c>
       <c r="BC13">
-        <v>110</v>
+        <v>516</v>
       </c>
       <c r="BD13">
-        <v>111</v>
+        <v>521</v>
       </c>
       <c r="BE13">
-        <v>112</v>
+        <v>528</v>
       </c>
       <c r="BF13">
-        <v>114</v>
+        <v>538</v>
       </c>
       <c r="BG13">
-        <v>117</v>
+        <v>542</v>
       </c>
       <c r="BH13">
-        <v>119</v>
+        <v>552</v>
       </c>
       <c r="BI13">
-        <v>120</v>
+        <v>560</v>
       </c>
       <c r="BJ13">
-        <v>123</v>
+        <v>565</v>
       </c>
       <c r="BK13">
-        <v>124</v>
+        <v>569</v>
       </c>
       <c r="BL13">
-        <v>127</v>
+        <v>574</v>
       </c>
       <c r="BM13">
-        <v>129</v>
+        <v>579</v>
       </c>
       <c r="BN13">
-        <v>129</v>
+        <v>583</v>
       </c>
       <c r="BO13">
-        <v>130</v>
+        <v>589</v>
       </c>
       <c r="BP13">
-        <v>132</v>
+        <v>595</v>
       </c>
       <c r="BQ13">
-        <v>132</v>
+        <v>601</v>
       </c>
       <c r="BR13">
-        <v>135</v>
+        <v>609</v>
       </c>
       <c r="BS13">
-        <v>137</v>
+        <v>612</v>
       </c>
       <c r="BT13">
-        <v>137</v>
+        <v>614</v>
       </c>
       <c r="BU13">
-        <v>139</v>
+        <v>620</v>
       </c>
       <c r="BV13">
-        <v>139</v>
+        <v>620</v>
       </c>
       <c r="BW13">
-        <v>142</v>
+        <v>624</v>
       </c>
       <c r="BX13">
-        <v>143</v>
+        <v>626</v>
       </c>
       <c r="BY13">
-        <v>145</v>
+        <v>631</v>
       </c>
       <c r="BZ13">
-        <v>145</v>
+        <v>631</v>
       </c>
     </row>
   </sheetData>

</xml_diff>